<commit_message>
Working worker and Scheduler
</commit_message>
<xml_diff>
--- a/tacomia.xlsx
+++ b/tacomia.xlsx
@@ -1105,7 +1105,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1135,54 +1135,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Pork Alarm</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>90</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Chef Hat</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>180</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Viking Helmet</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>300</v>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" t="n">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Rewrite Shopping and added dynamic day customer total
</commit_message>
<xml_diff>
--- a/tacomia.xlsx
+++ b/tacomia.xlsx
@@ -1421,7 +1421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1451,6 +1451,566 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Taco Hat</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>60</v>
+      </c>
+      <c r="C2" t="n">
+        <v>31</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Gold Spatula</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>100</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Gold Knife</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sombrero</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>120</v>
+      </c>
+      <c r="C5" t="n">
+        <v>32</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Extra Burner</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>150</v>
+      </c>
+      <c r="C6" t="n">
+        <v>28</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Extra Burner 2</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>200</v>
+      </c>
+      <c r="C7" t="n">
+        <v>29</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Small Plant</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>13</v>
+      </c>
+      <c r="C8" t="n">
+        <v>16</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hard Taco Sign</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>25</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Soft Taco Sign</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>25</v>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Pita Sign</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>25</v>
+      </c>
+      <c r="C11" t="n">
+        <v>6</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Chef Hat</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>180</v>
+      </c>
+      <c r="C12" t="n">
+        <v>33</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Romano Poster</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>50</v>
+      </c>
+      <c r="C13" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Viking Helmet</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>300</v>
+      </c>
+      <c r="C14" t="n">
+        <v>34</v>
+      </c>
+      <c r="D14" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Beans Poster</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>8</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Cactus</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>10</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mystery Poster</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>20</v>
+      </c>
+      <c r="C17" t="n">
+        <v>10</v>
+      </c>
+      <c r="D17" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Burgeria Poster</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>20</v>
+      </c>
+      <c r="C18" t="n">
+        <v>11</v>
+      </c>
+      <c r="D18" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Desert Plant</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>25</v>
+      </c>
+      <c r="C19" t="n">
+        <v>15</v>
+      </c>
+      <c r="D19" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Leafy Plant</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>40</v>
+      </c>
+      <c r="C20" t="n">
+        <v>17</v>
+      </c>
+      <c r="D20" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Onion Ring Poster</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>50</v>
+      </c>
+      <c r="C21" t="n">
+        <v>13</v>
+      </c>
+      <c r="D21" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Pepper Lights</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>60</v>
+      </c>
+      <c r="C22" t="n">
+        <v>7</v>
+      </c>
+      <c r="D22" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Coffee Stand</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>65</v>
+      </c>
+      <c r="C23" t="n">
+        <v>23</v>
+      </c>
+      <c r="D23" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Newspaper Stand</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>80</v>
+      </c>
+      <c r="C24" t="n">
+        <v>19</v>
+      </c>
+      <c r="D24" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Hypno Clock</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>80</v>
+      </c>
+      <c r="C25" t="n">
+        <v>30</v>
+      </c>
+      <c r="D25" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Gumball Machine</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>120</v>
+      </c>
+      <c r="C26" t="n">
+        <v>21</v>
+      </c>
+      <c r="D26" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Ceiling Fan</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>150</v>
+      </c>
+      <c r="C27" t="n">
+        <v>14</v>
+      </c>
+      <c r="D27" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>150</v>
+      </c>
+      <c r="C28" t="n">
+        <v>18</v>
+      </c>
+      <c r="D28" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Arcade Cabinet</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>400</v>
+      </c>
+      <c r="C29" t="n">
+        <v>20</v>
+      </c>
+      <c r="D29" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Jukebox</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>500</v>
+      </c>
+      <c r="C30" t="n">
+        <v>22</v>
+      </c>
+      <c r="D30" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Royal Crown</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C31" t="n">
+        <v>35</v>
+      </c>
+      <c r="D31" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Doorbell</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Beef Alarm</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>90</v>
+      </c>
+      <c r="C33" t="n">
+        <v>24</v>
+      </c>
+      <c r="D33" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Chicken Alarm</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>90</v>
+      </c>
+      <c r="C34" t="n">
+        <v>25</v>
+      </c>
+      <c r="D34" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Pork Alarm</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>90</v>
+      </c>
+      <c r="C35" t="n">
+        <v>26</v>
+      </c>
+      <c r="D35" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Steak Alarm</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>90</v>
+      </c>
+      <c r="C36" t="n">
+        <v>27</v>
+      </c>
+      <c r="D36" t="n">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>